<commit_message>
Combo Box Fund Bug Removed.
</commit_message>
<xml_diff>
--- a/bin/Debug/netcoreapp3.1/FundMarketSummary.xlsx
+++ b/bin/Debug/netcoreapp3.1/FundMarketSummary.xlsx
@@ -59,14 +59,14 @@
     <t>25,045</t>
   </si>
   <si>
-    <t xml:space="preserve">20.45
-</t>
-  </si>
-  <si>
-    <t>11,370</t>
-  </si>
-  <si>
-    <t>(13,675)</t>
+    <t xml:space="preserve">20.57
+</t>
+  </si>
+  <si>
+    <t>11,437</t>
+  </si>
+  <si>
+    <t>(13,608)</t>
   </si>
   <si>
     <t>At Tahur Limited</t>
@@ -84,14 +84,14 @@
     <t>7,820,772</t>
   </si>
   <si>
-    <t xml:space="preserve">20.90
-</t>
-  </si>
-  <si>
-    <t>9,321,400</t>
-  </si>
-  <si>
-    <t>1,500,628</t>
+    <t xml:space="preserve">21.03
+</t>
+  </si>
+  <si>
+    <t>9,379,380</t>
+  </si>
+  <si>
+    <t>1,558,608</t>
   </si>
   <si>
     <t>Attock Cement Pakistan Limited</t>
@@ -109,14 +109,14 @@
     <t>19,845,476</t>
   </si>
   <si>
-    <t xml:space="preserve">162.50
-</t>
-  </si>
-  <si>
-    <t>25,350,000</t>
-  </si>
-  <si>
-    <t>5,504,524</t>
+    <t xml:space="preserve">167.42
+</t>
+  </si>
+  <si>
+    <t>26,117,520</t>
+  </si>
+  <si>
+    <t>6,272,044</t>
   </si>
   <si>
     <t>Bankislami Pakistan Ltd.</t>
@@ -134,14 +134,14 @@
     <t>26,252</t>
   </si>
   <si>
-    <t xml:space="preserve">10.62
-</t>
-  </si>
-  <si>
-    <t>21,240</t>
-  </si>
-  <si>
-    <t>(5,012)</t>
+    <t xml:space="preserve">10.66
+</t>
+  </si>
+  <si>
+    <t>21,320</t>
+  </si>
+  <si>
+    <t>(4,932)</t>
   </si>
   <si>
     <t>Century Paper &amp; Board Mills</t>
@@ -159,14 +159,14 @@
     <t>20,300,902</t>
   </si>
   <si>
-    <t xml:space="preserve">113.15
-</t>
-  </si>
-  <si>
-    <t>32,247,750</t>
-  </si>
-  <si>
-    <t>11,946,848</t>
+    <t xml:space="preserve">115.07
+</t>
+  </si>
+  <si>
+    <t>32,794,950</t>
+  </si>
+  <si>
+    <t>12,494,048</t>
   </si>
   <si>
     <t>Cherat Cement Company Limited</t>
@@ -184,14 +184,14 @@
     <t>33,046,320</t>
   </si>
   <si>
-    <t xml:space="preserve">131.39
-</t>
-  </si>
-  <si>
-    <t>45,395,245</t>
-  </si>
-  <si>
-    <t>12,348,925</t>
+    <t xml:space="preserve">130.24
+</t>
+  </si>
+  <si>
+    <t>44,997,920</t>
+  </si>
+  <si>
+    <t>11,951,600</t>
   </si>
   <si>
     <t>D. G. Khan Cement</t>
@@ -209,14 +209,14 @@
     <t>62,057,378</t>
   </si>
   <si>
-    <t xml:space="preserve">112.80
-</t>
-  </si>
-  <si>
-    <t>81,795,792</t>
-  </si>
-  <si>
-    <t>19,738,414</t>
+    <t xml:space="preserve">112.83
+</t>
+  </si>
+  <si>
+    <t>81,817,546</t>
+  </si>
+  <si>
+    <t>19,760,169</t>
   </si>
   <si>
     <t>Dawood Hercules Corporation Limited</t>
@@ -234,14 +234,14 @@
     <t>582,193</t>
   </si>
   <si>
-    <t xml:space="preserve">129.00
-</t>
-  </si>
-  <si>
-    <t>475,236</t>
-  </si>
-  <si>
-    <t>(106,957)</t>
+    <t xml:space="preserve">129.14
+</t>
+  </si>
+  <si>
+    <t>475,752</t>
+  </si>
+  <si>
+    <t>(106,442)</t>
   </si>
   <si>
     <t>Engro Corporation</t>
@@ -259,14 +259,14 @@
     <t>233,362,180</t>
   </si>
   <si>
-    <t xml:space="preserve">302.49
-</t>
-  </si>
-  <si>
-    <t>232,221,271</t>
-  </si>
-  <si>
-    <t>(1,140,909)</t>
+    <t xml:space="preserve">304.75
+</t>
+  </si>
+  <si>
+    <t>233,956,270</t>
+  </si>
+  <si>
+    <t>594,090</t>
   </si>
   <si>
     <t>Engro Fertilizer Limited</t>
@@ -284,14 +284,14 @@
     <t>101,589,373</t>
   </si>
   <si>
-    <t xml:space="preserve">61.48
-</t>
-  </si>
-  <si>
-    <t>94,488,182</t>
-  </si>
-  <si>
-    <t>(7,101,191)</t>
+    <t xml:space="preserve">61.74
+</t>
+  </si>
+  <si>
+    <t>94,887,774</t>
+  </si>
+  <si>
+    <t>(6,701,599)</t>
   </si>
   <si>
     <t>Engro Polymer &amp; Chemicals Limited</t>
@@ -309,14 +309,14 @@
     <t>32,595,635</t>
   </si>
   <si>
-    <t xml:space="preserve">44.90
-</t>
-  </si>
-  <si>
-    <t>48,716,500</t>
-  </si>
-  <si>
-    <t>16,120,865</t>
+    <t xml:space="preserve">44.93
+</t>
+  </si>
+  <si>
+    <t>48,749,050</t>
+  </si>
+  <si>
+    <t>16,153,415</t>
   </si>
   <si>
     <t>Fauji Cement</t>
@@ -334,14 +334,14 @@
     <t>2,734,246</t>
   </si>
   <si>
-    <t xml:space="preserve">21.19
-</t>
-  </si>
-  <si>
-    <t>3,146,715</t>
-  </si>
-  <si>
-    <t>412,469</t>
+    <t xml:space="preserve">21.13
+</t>
+  </si>
+  <si>
+    <t>3,137,805</t>
+  </si>
+  <si>
+    <t>403,559</t>
   </si>
   <si>
     <t>Fauji Fertilizer Company</t>
@@ -359,14 +359,14 @@
     <t>1,627,783</t>
   </si>
   <si>
-    <t xml:space="preserve">109.80
-</t>
-  </si>
-  <si>
-    <t>1,899,540</t>
-  </si>
-  <si>
-    <t>271,757</t>
+    <t xml:space="preserve">109.99
+</t>
+  </si>
+  <si>
+    <t>1,902,827</t>
+  </si>
+  <si>
+    <t>275,044</t>
   </si>
   <si>
     <t>Ferozsons Laboratory Limited</t>
@@ -409,14 +409,14 @@
     <t>1,170,570</t>
   </si>
   <si>
-    <t xml:space="preserve">185.90
-</t>
-  </si>
-  <si>
-    <t>1,338,480</t>
-  </si>
-  <si>
-    <t>167,910</t>
+    <t xml:space="preserve">185.89
+</t>
+  </si>
+  <si>
+    <t>1,338,408</t>
+  </si>
+  <si>
+    <t>167,838</t>
   </si>
   <si>
     <t>Hascol Petroleum</t>
@@ -434,14 +434,14 @@
     <t>26,127,844</t>
   </si>
   <si>
-    <t xml:space="preserve">21.09
-</t>
-  </si>
-  <si>
-    <t>38,768,482</t>
-  </si>
-  <si>
-    <t>12,640,637</t>
+    <t xml:space="preserve">21.08
+</t>
+  </si>
+  <si>
+    <t>38,750,099</t>
+  </si>
+  <si>
+    <t>12,622,255</t>
   </si>
   <si>
     <t>Highnoon (Lab)</t>
@@ -459,7 +459,7 @@
     <t>47,798,829</t>
   </si>
   <si>
-    <t xml:space="preserve">628.00
+    <t xml:space="preserve">628
 </t>
   </si>
   <si>
@@ -484,14 +484,14 @@
     <t>9,385,593</t>
   </si>
   <si>
-    <t xml:space="preserve">303.00
-</t>
-  </si>
-  <si>
-    <t>13,847,100</t>
-  </si>
-  <si>
-    <t>4,461,507</t>
+    <t xml:space="preserve">304.89
+</t>
+  </si>
+  <si>
+    <t>13,933,473</t>
+  </si>
+  <si>
+    <t>4,547,880</t>
   </si>
   <si>
     <t>Hub Power Company</t>
@@ -509,14 +509,14 @@
     <t>131,231,845</t>
   </si>
   <si>
-    <t xml:space="preserve">80.70
-</t>
-  </si>
-  <si>
-    <t>118,120,186</t>
-  </si>
-  <si>
-    <t>(13,111,658)</t>
+    <t xml:space="preserve">81.26
+</t>
+  </si>
+  <si>
+    <t>118,939,856</t>
+  </si>
+  <si>
+    <t>(12,291,989)</t>
   </si>
   <si>
     <t>ICI Pakistan Limited</t>
@@ -583,14 +583,14 @@
     <t>10,984,402</t>
   </si>
   <si>
-    <t xml:space="preserve">154.00
-</t>
-  </si>
-  <si>
-    <t>17,093,384</t>
-  </si>
-  <si>
-    <t>6,108,982</t>
+    <t xml:space="preserve">154.50
+</t>
+  </si>
+  <si>
+    <t>17,148,882</t>
+  </si>
+  <si>
+    <t>6,164,480</t>
   </si>
   <si>
     <t>International Steels Limited</t>
@@ -608,14 +608,14 @@
     <t>14,145,453</t>
   </si>
   <si>
-    <t xml:space="preserve">79.55
-</t>
-  </si>
-  <si>
-    <t>22,228,577</t>
-  </si>
-  <si>
-    <t>8,083,123</t>
+    <t xml:space="preserve">79.63
+</t>
+  </si>
+  <si>
+    <t>22,250,931</t>
+  </si>
+  <si>
+    <t>8,105,478</t>
   </si>
   <si>
     <t>Ittehad Chemicals Ltd</t>
@@ -633,14 +633,14 @@
     <t>12,131,403</t>
   </si>
   <si>
-    <t xml:space="preserve">29.00
-</t>
-  </si>
-  <si>
-    <t>14,152,000</t>
-  </si>
-  <si>
-    <t>2,020,597</t>
+    <t xml:space="preserve">29.14
+</t>
+  </si>
+  <si>
+    <t>14,220,320</t>
+  </si>
+  <si>
+    <t>2,088,917</t>
   </si>
   <si>
     <t>K-Electric Limited</t>
@@ -683,7 +683,7 @@
     <t>12,451,110</t>
   </si>
   <si>
-    <t xml:space="preserve">200.00
+    <t xml:space="preserve">200
 </t>
   </si>
   <si>
@@ -708,14 +708,14 @@
     <t>41,911,613</t>
   </si>
   <si>
-    <t xml:space="preserve">61.00
-</t>
-  </si>
-  <si>
-    <t>63,028,311</t>
-  </si>
-  <si>
-    <t>21,116,698</t>
+    <t xml:space="preserve">60.54
+</t>
+  </si>
+  <si>
+    <t>62,553,016</t>
+  </si>
+  <si>
+    <t>20,641,403</t>
   </si>
   <si>
     <t xml:space="preserve">Lotte Chemical Pakistan Ltd </t>
@@ -733,14 +733,14 @@
     <t>21,126,686</t>
   </si>
   <si>
-    <t xml:space="preserve">12.52
-</t>
-  </si>
-  <si>
-    <t>24,270,020</t>
-  </si>
-  <si>
-    <t>3,143,334</t>
+    <t xml:space="preserve">12.69
+</t>
+  </si>
+  <si>
+    <t>24,599,565</t>
+  </si>
+  <si>
+    <t>3,472,879</t>
   </si>
   <si>
     <t>Lucky Cement</t>
@@ -758,14 +758,14 @@
     <t>159,240,184</t>
   </si>
   <si>
-    <t xml:space="preserve">661.00
-</t>
-  </si>
-  <si>
-    <t>237,938,848</t>
-  </si>
-  <si>
-    <t>78,698,664</t>
+    <t xml:space="preserve">662.86
+</t>
+  </si>
+  <si>
+    <t>238,608,388</t>
+  </si>
+  <si>
+    <t>79,368,205</t>
   </si>
   <si>
     <t>Maple Leaf Cement Factory Limited</t>
@@ -783,14 +783,14 @@
     <t>44,922,183</t>
   </si>
   <si>
-    <t xml:space="preserve">39.80
-</t>
-  </si>
-  <si>
-    <t>66,392,768</t>
-  </si>
-  <si>
-    <t>21,470,585</t>
+    <t xml:space="preserve">39.70
+</t>
+  </si>
+  <si>
+    <t>66,225,952</t>
+  </si>
+  <si>
+    <t>21,303,769</t>
   </si>
   <si>
     <t>Mari Petroleum Co. Ltd</t>
@@ -826,14 +826,14 @@
     <t>93,959,562</t>
   </si>
   <si>
-    <t xml:space="preserve">80.88
-</t>
-  </si>
-  <si>
-    <t>101,783,840</t>
-  </si>
-  <si>
-    <t>7,824,279</t>
+    <t xml:space="preserve">80.23
+</t>
+  </si>
+  <si>
+    <t>100,965,845</t>
+  </si>
+  <si>
+    <t>7,006,283</t>
   </si>
   <si>
     <t>Millat Tractors</t>
@@ -851,14 +851,14 @@
     <t>45,447,667</t>
   </si>
   <si>
-    <t xml:space="preserve">878.00
-</t>
-  </si>
-  <si>
-    <t>45,639,318</t>
-  </si>
-  <si>
-    <t>191,651</t>
+    <t xml:space="preserve">879.55
+</t>
+  </si>
+  <si>
+    <t>45,719,889</t>
+  </si>
+  <si>
+    <t>272,221</t>
   </si>
   <si>
     <t>Mughal Iron &amp; Steel Industries</t>
@@ -876,14 +876,14 @@
     <t>20,634,240</t>
   </si>
   <si>
-    <t xml:space="preserve">68.25
-</t>
-  </si>
-  <si>
-    <t>29,518,125</t>
-  </si>
-  <si>
-    <t>8,883,885</t>
+    <t xml:space="preserve">68.12
+</t>
+  </si>
+  <si>
+    <t>29,461,900</t>
+  </si>
+  <si>
+    <t>8,827,660</t>
   </si>
   <si>
     <t>Nishat Mills Limited</t>
@@ -901,14 +901,14 @@
     <t>71,341,773</t>
   </si>
   <si>
-    <t xml:space="preserve">105.25
-</t>
-  </si>
-  <si>
-    <t>77,724,388</t>
-  </si>
-  <si>
-    <t>6,382,615</t>
+    <t xml:space="preserve">105.04
+</t>
+  </si>
+  <si>
+    <t>77,569,309</t>
+  </si>
+  <si>
+    <t>6,227,536</t>
   </si>
   <si>
     <t>Oil &amp; Gas Development Company Limited</t>
@@ -926,14 +926,14 @@
     <t>232,760,985</t>
   </si>
   <si>
-    <t xml:space="preserve">104.70
-</t>
-  </si>
-  <si>
-    <t>193,051,618</t>
-  </si>
-  <si>
-    <t>(39,709,366)</t>
+    <t xml:space="preserve">104.94
+</t>
+  </si>
+  <si>
+    <t>193,494,144</t>
+  </si>
+  <si>
+    <t>(39,266,841)</t>
   </si>
   <si>
     <t>Pak Suzuki Motor Company</t>
@@ -951,14 +951,14 @@
     <t>19,843,137</t>
   </si>
   <si>
-    <t xml:space="preserve">221.00
-</t>
-  </si>
-  <si>
-    <t>22,895,600</t>
-  </si>
-  <si>
-    <t>3,052,463</t>
+    <t xml:space="preserve">224.11
+</t>
+  </si>
+  <si>
+    <t>23,217,796</t>
+  </si>
+  <si>
+    <t>3,374,659</t>
   </si>
   <si>
     <t>Pakistan National Shipping Co.</t>
@@ -976,14 +976,14 @@
     <t>23,196,890</t>
   </si>
   <si>
-    <t xml:space="preserve">90.00
-</t>
-  </si>
-  <si>
-    <t>25,785,000</t>
-  </si>
-  <si>
-    <t>2,588,110</t>
+    <t xml:space="preserve">90.40
+</t>
+  </si>
+  <si>
+    <t>25,899,600</t>
+  </si>
+  <si>
+    <t>2,702,710</t>
   </si>
   <si>
     <t>Pakistan Oilfields Limited</t>
@@ -1001,14 +1001,14 @@
     <t>98,298,528</t>
   </si>
   <si>
-    <t xml:space="preserve">423.00
-</t>
-  </si>
-  <si>
-    <t>101,842,749</t>
-  </si>
-  <si>
-    <t>3,544,221</t>
+    <t xml:space="preserve">424.10
+</t>
+  </si>
+  <si>
+    <t>102,107,588</t>
+  </si>
+  <si>
+    <t>3,809,060</t>
   </si>
   <si>
     <t>Pakistan Petroleum Limited</t>
@@ -1026,14 +1026,14 @@
     <t>230,834,179</t>
   </si>
   <si>
-    <t xml:space="preserve">93.40
-</t>
-  </si>
-  <si>
-    <t>195,366,088</t>
-  </si>
-  <si>
-    <t>(35,468,092)</t>
+    <t xml:space="preserve">92.88
+</t>
+  </si>
+  <si>
+    <t>194,278,396</t>
+  </si>
+  <si>
+    <t>(36,555,783)</t>
   </si>
   <si>
     <t>Pakistan State Oil</t>
@@ -1051,14 +1051,14 @@
     <t>114,247,038</t>
   </si>
   <si>
-    <t xml:space="preserve">202.51
-</t>
-  </si>
-  <si>
-    <t>129,682,341</t>
-  </si>
-  <si>
-    <t>15,435,303</t>
+    <t xml:space="preserve">205.62
+</t>
+  </si>
+  <si>
+    <t>131,673,908</t>
+  </si>
+  <si>
+    <t>17,426,869</t>
   </si>
   <si>
     <t>Pioneer Cement</t>
@@ -1076,14 +1076,14 @@
     <t>18,343,446</t>
   </si>
   <si>
-    <t xml:space="preserve">98.84
-</t>
-  </si>
-  <si>
-    <t>33,803,280</t>
-  </si>
-  <si>
-    <t>15,459,834</t>
+    <t xml:space="preserve">98.23
+</t>
+  </si>
+  <si>
+    <t>33,594,660</t>
+  </si>
+  <si>
+    <t>15,251,214</t>
   </si>
   <si>
     <t>Sui Northern Gas Pipelines Limited</t>
@@ -1126,14 +1126,14 @@
     <t>580,169</t>
   </si>
   <si>
-    <t xml:space="preserve">48.30
-</t>
-  </si>
-  <si>
-    <t>477,639</t>
-  </si>
-  <si>
-    <t>(102,531)</t>
+    <t xml:space="preserve">47.93
+</t>
+  </si>
+  <si>
+    <t>473,980</t>
+  </si>
+  <si>
+    <t>(106,190)</t>
   </si>
   <si>
     <t>Systems Limited</t>
@@ -1151,14 +1151,14 @@
     <t>47,692,858</t>
   </si>
   <si>
-    <t xml:space="preserve">298.53
-</t>
-  </si>
-  <si>
-    <t>118,089,512</t>
-  </si>
-  <si>
-    <t>70,396,655</t>
+    <t xml:space="preserve">299.48
+</t>
+  </si>
+  <si>
+    <t>118,465,304</t>
+  </si>
+  <si>
+    <t>70,772,446</t>
   </si>
   <si>
     <t>THAL LIMITED</t>
@@ -1176,14 +1176,14 @@
     <t>31,294,637</t>
   </si>
   <si>
-    <t xml:space="preserve">411.00
-</t>
-  </si>
-  <si>
-    <t>39,127,200</t>
-  </si>
-  <si>
-    <t>7,832,563</t>
+    <t xml:space="preserve">426.01
+</t>
+  </si>
+  <si>
+    <t>40,556,152</t>
+  </si>
+  <si>
+    <t>9,261,515</t>
   </si>
   <si>
     <t>The Organic Meat Company Limited</t>
@@ -1201,14 +1201,14 @@
     <t>1,050,480</t>
   </si>
   <si>
-    <t xml:space="preserve">30.25
-</t>
-  </si>
-  <si>
-    <t>1,588,851</t>
-  </si>
-  <si>
-    <t>538,371</t>
+    <t xml:space="preserve">31.38
+</t>
+  </si>
+  <si>
+    <t>1,648,203</t>
+  </si>
+  <si>
+    <t>597,723</t>
   </si>
   <si>
     <t>The Searle Company</t>
@@ -1226,14 +1226,14 @@
     <t>64,601,698</t>
   </si>
   <si>
-    <t xml:space="preserve">273.00
-</t>
-  </si>
-  <si>
-    <t>76,377,483</t>
-  </si>
-  <si>
-    <t>11,775,785</t>
+    <t xml:space="preserve">271.38
+</t>
+  </si>
+  <si>
+    <t>75,924,254</t>
+  </si>
+  <si>
+    <t>11,322,556</t>
   </si>
   <si>
     <t>Unity Foods Limited</t>
@@ -1251,14 +1251,14 @@
     <t>12,924,125</t>
   </si>
   <si>
-    <t xml:space="preserve">18.09
-</t>
-  </si>
-  <si>
-    <t>21,916,035</t>
-  </si>
-  <si>
-    <t>8,991,910</t>
+    <t xml:space="preserve">18.04
+</t>
+  </si>
+  <si>
+    <t>21,855,460</t>
+  </si>
+  <si>
+    <t>8,931,335</t>
   </si>
   <si>
     <t>Unity Foods Limited(R2)</t>

</xml_diff>